<commit_message>
updated topic: datasets and dicionario_de_dados
</commit_message>
<xml_diff>
--- a/dataset/Bancos.xlsx
+++ b/dataset/Bancos.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34ed68c2d0e7e9fe/YouTube/2024-05-12 - Fluxo de caixa/Projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Documents\_rma\_tecnologia\_data\evolve_data\projetos\projeto_fluxo_de_caixa_evolve\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_AD4D361C20488DEA4E38A01D8C1A674C5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{174E2082-9C48-4874-B6A8-4E43623B0382}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B35113-9C21-4CE8-A8F8-CE423E7E3279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bancos" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Banco_ID</t>
   </si>
@@ -40,13 +41,77 @@
   </si>
   <si>
     <t>Inter</t>
+  </si>
+  <si>
+    <t>Coluna</t>
+  </si>
+  <si>
+    <t>Tipo de Dado</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <r>
+      <t>Inteiro (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>int64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Identificador único de cada banco. Utilizado como chave primária para relacionamentos.</t>
+  </si>
+  <si>
+    <r>
+      <t>Texto (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Nome do banco correspondente ao identificador. Ex.: Itaú Unibanco, Bradesco, Inter.</t>
+  </si>
+  <si>
+    <t>Tabela: Bancos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +119,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,12 +155,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,13 +489,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,7 +503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -394,7 +511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -402,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -416,4 +533,60 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDF74BD-7E63-4815-B032-5A6E16138C0D}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="40.5" customHeight="1">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="40.5" customHeight="1">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>